<commit_message>
mend the equip effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/EquipAddon.xlsx
+++ b/ConfigData/Xlsx/EquipAddon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>attr</t>
   </si>
@@ -71,15 +71,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>生命+{0}</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>攻击</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>攻击+{0}</t>
+    <t>防御塔攻击+{0}%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御塔生命+{0}%</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>射速</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>射程</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御塔射速+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御塔射程+{0}</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -755,6 +771,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -767,8 +851,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E7" totalsRowShown="0">
+  <autoFilter ref="A1:E7"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
@@ -788,7 +872,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CAEACD"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1067,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1135,10 +1219,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1155,13 +1239,47 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
balance the equip data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/EquipAddon.xlsx
+++ b/ConfigData/Xlsx/EquipAddon.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -14,15 +14,12 @@
   <sheets>
     <sheet name="EquipAddon" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
-  <si>
-    <t>attr</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -70,15 +67,9 @@
     <t>攻击</t>
   </si>
   <si>
-    <t>防御塔攻击+{0}%</t>
-  </si>
-  <si>
     <t>生命</t>
   </si>
   <si>
-    <t>防御塔生命+{0}%</t>
-  </si>
-  <si>
     <t>射速</t>
   </si>
   <si>
@@ -125,13 +116,186 @@
   </si>
   <si>
     <t>防御塔幸运+{0}</t>
+  </si>
+  <si>
+    <t>防御塔攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御塔生命+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>防御</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻速</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>命中</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>回避</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>暴击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>幸运</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtkP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>VitP</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Def</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mag</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dhit</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crt</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Luk</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>射程</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物选取</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EquipMonsterPickDelegate</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>PickMethod</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Human")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Undead")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Orc")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Spirit")</t>
+  </si>
+  <si>
+    <t>m.Star&gt;0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Beast")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Machine") || m.Action.IsRace("Element")</t>
+  </si>
+  <si>
+    <t>m.Action.IsRace("Totem") || m.Action.IsRace("Element")</t>
+  </si>
+  <si>
+    <t>m.Star&gt;5</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方人类生命+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方亡灵攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方兽人攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方精灵生命+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方所有单位生命+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方所有单位攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方野兽攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方机械和元素攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方图腾和元素攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>我方5星以上单位攻击+{0}</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>double</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,8 +473,17 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +666,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,7 +975,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -792,6 +995,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -839,7 +1066,15 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -921,14 +1156,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:E13" totalsRowShown="0">
-  <autoFilter ref="A3:E13"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A3:P23" totalsRowShown="0">
+  <autoFilter ref="A3:P23"/>
+  <tableColumns count="16">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="3" name="Format"/>
     <tableColumn id="4" name="Type"/>
     <tableColumn id="5" name="Rare"/>
+    <tableColumn id="16" name="PickMethod"/>
+    <tableColumn id="6" name="AtkP"/>
+    <tableColumn id="7" name="VitP"/>
+    <tableColumn id="15" name="Range"/>
+    <tableColumn id="8" name="Def"/>
+    <tableColumn id="9" name="Mag"/>
+    <tableColumn id="10" name="Spd"/>
+    <tableColumn id="11" name="Hit"/>
+    <tableColumn id="12" name="Dhit"/>
+    <tableColumn id="13" name="Crt"/>
+    <tableColumn id="14" name="Luk"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1255,240 +1501,611 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="28.125" customWidth="1"/>
+    <col min="4" max="5" width="4.875" customWidth="1"/>
+    <col min="6" max="6" width="23.125" customWidth="1"/>
+    <col min="7" max="16" width="5.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="55.5" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13">
         <v>2</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A14">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.15">
+      <c r="A16">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A21">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A22">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A23">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="F14:F23">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(F14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>